<commit_message>
created a protocol for preperation of 0.02M pbs
</commit_message>
<xml_diff>
--- a/Chemichals, Solutions, Dlutions, and Reagents/DoseCalculator.xlsx
+++ b/Chemichals, Solutions, Dlutions, and Reagents/DoseCalculator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idobe\Documents\GitHub\lab-handbook\Chemichals, Solutions, Dlutions, and Reagents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96AFA93C-3638-45A3-ABAD-B488F1596006}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C87098E6-E374-4371-BC21-ADC8A2DCB5C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21000" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23745" yWindow="0" windowWidth="14655" windowHeight="21000" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Midazolam" sheetId="5" r:id="rId1"/>
@@ -532,7 +532,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D9">
-        <v>0.25</v>
+        <v>0.04</v>
       </c>
       <c r="E9" t="s">
         <v>7</v>
@@ -544,7 +544,7 @@
       </c>
       <c r="D10">
         <f>D9*D8</f>
-        <v>1.25</v>
+        <v>0.2</v>
       </c>
       <c r="E10" t="s">
         <v>6</v>
@@ -556,7 +556,7 @@
       </c>
       <c r="D11">
         <f>D6/D10</f>
-        <v>3.5999999999999997E-2</v>
+        <v>0.22499999999999998</v>
       </c>
       <c r="E11" t="s">
         <v>9</v>
@@ -618,7 +618,7 @@
         <v>3</v>
       </c>
       <c r="D5">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E5" t="s">
         <v>2</v>
@@ -630,7 +630,7 @@
       </c>
       <c r="D6">
         <f>D5*D4</f>
-        <v>1.4000000000000001</v>
+        <v>1.5</v>
       </c>
       <c r="E6" t="s">
         <v>4</v>
@@ -649,7 +649,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D9">
-        <v>0.25</v>
+        <v>0.04</v>
       </c>
       <c r="E9" t="s">
         <v>7</v>
@@ -661,7 +661,7 @@
       </c>
       <c r="D10">
         <f>D9*D8</f>
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="E10" t="s">
         <v>6</v>
@@ -673,7 +673,7 @@
       </c>
       <c r="D11">
         <f>D6/D10</f>
-        <v>5.6000000000000008E-2</v>
+        <v>0.375</v>
       </c>
       <c r="E11" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
added Ketamine Midazolam tabs
ketamin and midazolam dosages can now be calculated using this excel file
</commit_message>
<xml_diff>
--- a/Chemichals, Solutions, Dlutions, and Reagents/DoseCalculator.xlsx
+++ b/Chemichals, Solutions, Dlutions, and Reagents/DoseCalculator.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Yardenc/Documents/GitHub/lab-handbook/Chemichals, Solutions, Dlutions, and Reagents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idobe\Documents\GitHub\Ido_lab-handbook\Chemichals, Solutions, Dlutions, and Reagents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{410D48A6-E653-4449-93E7-A350C4DD3D5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{927010F1-ADA3-4D8C-AB07-E673CA402AED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4520" yWindow="760" windowWidth="25720" windowHeight="17920" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Meloxicam" sheetId="1" r:id="rId1"/>
     <sheet name="Pentobarbital" sheetId="2" r:id="rId2"/>
     <sheet name="Lidocaine" sheetId="3" r:id="rId3"/>
+    <sheet name="Ketamin" sheetId="5" r:id="rId4"/>
+    <sheet name="Midazolam" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="28">
   <si>
     <t>mg/kg</t>
   </si>
@@ -110,6 +112,18 @@
   </si>
   <si>
     <t>Inject 0.1-0.15ml since birds are smaller</t>
+  </si>
+  <si>
+    <t>Concentration of Ketamin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ketamin 150mg/kg </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Midazolam  1.5mg/kg </t>
+  </si>
+  <si>
+    <t>Concentration of Midazolam</t>
   </si>
 </sst>
 </file>
@@ -464,21 +478,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="A3" sqref="A3:E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:5" ht="33" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="33" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D4" s="1" t="s">
         <v>13</v>
       </c>
@@ -486,7 +500,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>11</v>
       </c>
@@ -497,7 +511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D6">
         <f>D5/1000</f>
         <v>5.0000000000000001E-4</v>
@@ -506,7 +520,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>3</v>
       </c>
@@ -517,7 +531,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>5</v>
       </c>
@@ -529,7 +543,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="3" t="s">
         <v>15</v>
       </c>
@@ -540,7 +554,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D11">
         <v>0.01</v>
       </c>
@@ -548,7 +562,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>8</v>
       </c>
@@ -560,7 +574,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="24" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
       <c r="C13" s="4" t="s">
         <v>16</v>
       </c>
@@ -572,7 +586,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>10</v>
       </c>
@@ -583,7 +597,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D16">
         <v>0.01</v>
       </c>
@@ -591,7 +605,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>8</v>
       </c>
@@ -603,7 +617,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="3:5" ht="24" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:5" ht="23.25" x14ac:dyDescent="0.35">
       <c r="C18" s="4" t="s">
         <v>17</v>
       </c>
@@ -628,17 +642,17 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="15.1640625" customWidth="1"/>
+    <col min="3" max="3" width="15.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="33" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="33" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D2" s="1" t="s">
         <v>13</v>
       </c>
@@ -646,7 +660,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>11</v>
       </c>
@@ -657,7 +671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D4">
         <f>D3/1000</f>
         <v>0.14000000000000001</v>
@@ -666,7 +680,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>3</v>
       </c>
@@ -677,7 +691,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>5</v>
       </c>
@@ -689,7 +703,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C8" s="3" t="s">
         <v>21</v>
       </c>
@@ -700,7 +714,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D9">
         <v>0.1</v>
       </c>
@@ -708,7 +722,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>8</v>
       </c>
@@ -720,7 +734,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="24" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
       <c r="C11" s="4" t="s">
         <v>16</v>
       </c>
@@ -741,21 +755,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F9B0A0D-DFB3-9642-870B-F8FEA932FE1C}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="45.1640625" customWidth="1"/>
+    <col min="3" max="3" width="45.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="33" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="33" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D2" s="1" t="s">
         <v>13</v>
       </c>
@@ -763,7 +777,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>11</v>
       </c>
@@ -774,7 +788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D4">
         <f>D3/1000</f>
         <v>2E-3</v>
@@ -783,7 +797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>3</v>
       </c>
@@ -794,7 +808,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>5</v>
       </c>
@@ -806,7 +820,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C8" s="3" t="s">
         <v>22</v>
       </c>
@@ -817,7 +831,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D9">
         <v>0.02</v>
       </c>
@@ -825,7 +839,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>8</v>
       </c>
@@ -837,7 +851,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="24" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
       <c r="C11" s="4" t="s">
         <v>20</v>
       </c>
@@ -849,10 +863,250 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C13" s="5" t="s">
         <v>23</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F27607E-051D-4736-AA21-60C05CFEC29B}">
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="45.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="33" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3">
+        <v>150</v>
+      </c>
+      <c r="E3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <f>D3/1000</f>
+        <v>0.15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>36</v>
+      </c>
+      <c r="E5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <f>D5*D4</f>
+        <v>5.3999999999999995</v>
+      </c>
+      <c r="E6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8">
+        <v>100</v>
+      </c>
+      <c r="E8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>0.2</v>
+      </c>
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10">
+        <f>D9*D8</f>
+        <v>20</v>
+      </c>
+      <c r="E10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C11" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11">
+        <f>D6/D10</f>
+        <v>0.26999999999999996</v>
+      </c>
+      <c r="E11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C13" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BD30AC6-3564-4096-A21C-BBCE22A30283}">
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="45.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="33" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3">
+        <v>1.5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <f>D3/1000</f>
+        <v>1.5E-3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>36</v>
+      </c>
+      <c r="E5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <f>D5*D4</f>
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8">
+        <v>5</v>
+      </c>
+      <c r="E8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>0.04</v>
+      </c>
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10">
+        <f>D9*D8</f>
+        <v>0.2</v>
+      </c>
+      <c r="E10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C11" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11">
+        <f>D6/D10</f>
+        <v>0.26999999999999996</v>
+      </c>
+      <c r="E11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C13" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>